<commit_message>
Update data package at: 2025-09-26T17:41:22Z
</commit_message>
<xml_diff>
--- a/data/sisor-dados/base_categoria_pessoal.xlsx
+++ b/data/sisor-dados/base_categoria_pessoal.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E339"/>
+  <dimension ref="A1:E332"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,11 +476,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>295</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -499,11 +499,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>32</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4">
@@ -522,11 +522,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>476</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5">
@@ -540,16 +540,16 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MEMBROS DE PODER</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>78</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="6">
@@ -591,11 +591,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>OUTRAS</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>74</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
@@ -609,16 +609,16 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>MEMBROS DE PODER</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1251</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9">
@@ -637,11 +637,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>OUTRAS</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>26</v>
+        <v>476</v>
       </c>
     </row>
     <row r="10">
@@ -683,11 +683,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>217</v>
+        <v>667</v>
       </c>
     </row>
     <row r="12">
@@ -752,11 +752,11 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>MEMBROS DE PODER</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>667</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
@@ -775,11 +775,11 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>MEMBROS DE PODER</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16">
@@ -793,16 +793,16 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>6977</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -844,11 +844,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>8557</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19">
@@ -862,16 +862,16 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>1161</v>
+        <v>6977</v>
       </c>
     </row>
     <row r="20">
@@ -890,11 +890,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>8557</v>
       </c>
     </row>
     <row r="21">
@@ -913,11 +913,11 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>MEMBROS DE PODER</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>110</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="22">
@@ -936,11 +936,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>MEMBROS DE PODER</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>1132</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="23">
@@ -959,11 +959,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>OUTRAS</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
@@ -977,16 +977,16 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>INATIVO MILITAR</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>10</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25">
@@ -1023,16 +1023,16 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>INATIVO MILITAR</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>77</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27">
@@ -1051,11 +1051,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>OUTRAS</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28">
@@ -1074,11 +1074,11 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>MEMBROS DE PODER</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29">
@@ -1120,11 +1120,11 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>MEMBROS DE PODER</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31">
@@ -1138,16 +1138,16 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>27</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32">
@@ -1161,16 +1161,16 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>60</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33">
@@ -1230,16 +1230,16 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>222</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36">
@@ -1253,16 +1253,16 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>53</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37">
@@ -1281,11 +1281,11 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>434</v>
+        <v>319</v>
       </c>
     </row>
     <row r="38">
@@ -1304,11 +1304,11 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>319</v>
+        <v>434</v>
       </c>
     </row>
     <row r="39">
@@ -1368,16 +1368,16 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>1483</v>
+        <v>483</v>
       </c>
     </row>
     <row r="42">
@@ -1437,16 +1437,16 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>483</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="45">
@@ -1465,11 +1465,11 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>41</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -1483,16 +1483,16 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47">
@@ -1506,16 +1506,16 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
@@ -1534,11 +1534,11 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49">
@@ -1557,11 +1557,11 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50">
@@ -1580,11 +1580,11 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51">
@@ -1603,11 +1603,11 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>570</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52">
@@ -1621,16 +1621,16 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>4293</v>
+        <v>767</v>
       </c>
     </row>
     <row r="53">
@@ -1644,16 +1644,16 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4293</v>
       </c>
     </row>
     <row r="54">
@@ -1672,11 +1672,11 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>767</v>
+        <v>570</v>
       </c>
     </row>
     <row r="55">
@@ -1718,11 +1718,11 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>133</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57">
@@ -1736,16 +1736,16 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>46</v>
+        <v>409</v>
       </c>
     </row>
     <row r="58">
@@ -1764,11 +1764,11 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>8</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59">
@@ -1782,16 +1782,16 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>409</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60">
@@ -1810,11 +1810,11 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>45</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61">
@@ -1828,16 +1828,16 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>481</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62">
@@ -1851,16 +1851,16 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>41</v>
+        <v>481</v>
       </c>
     </row>
     <row r="63">
@@ -1879,11 +1879,11 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>108</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64">
@@ -1902,11 +1902,11 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65">
@@ -1925,11 +1925,11 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>DOCENTE</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>2339</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
@@ -1948,11 +1948,11 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>1793</v>
+        <v>237</v>
       </c>
     </row>
     <row r="67">
@@ -1971,11 +1971,11 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>OFICIAL</t>
+          <t>NATUREZA ESPECIAL</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>3764</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -1994,11 +1994,11 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>PRAÇA</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>33828</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69">
@@ -2012,16 +2012,16 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>INATIVO MILITAR</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>190</v>
+        <v>39337</v>
       </c>
     </row>
     <row r="70">
@@ -2035,16 +2035,16 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>INATIVO MILITAR</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>39337</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="71">
@@ -2063,11 +2063,11 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>OFICIAL</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>3764</v>
       </c>
     </row>
     <row r="72">
@@ -2086,11 +2086,11 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>PRAÇA</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>237</v>
+        <v>33828</v>
       </c>
     </row>
     <row r="73">
@@ -2104,16 +2104,16 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>NATUREZA ESPECIAL</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>470</v>
       </c>
     </row>
     <row r="74">
@@ -2127,16 +2127,16 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>DOCENTE</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>470</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="75">
@@ -2155,11 +2155,11 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>DOCENTE</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>158968</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
@@ -2178,11 +2178,11 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>37607</v>
+        <v>4144</v>
       </c>
     </row>
     <row r="77">
@@ -2196,16 +2196,16 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>176055</v>
+        <v>23323</v>
       </c>
     </row>
     <row r="78">
@@ -2219,16 +2219,16 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>14014</v>
+        <v>176055</v>
       </c>
     </row>
     <row r="79">
@@ -2247,11 +2247,11 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>DOCENTE</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>4144</v>
+        <v>158968</v>
       </c>
     </row>
     <row r="80">
@@ -2270,11 +2270,11 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>23323</v>
+        <v>37607</v>
       </c>
     </row>
     <row r="81">
@@ -2293,11 +2293,11 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>6</v>
+        <v>14014</v>
       </c>
     </row>
     <row r="82">
@@ -2316,11 +2316,11 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83">
@@ -2339,11 +2339,11 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>OUTRAS</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84">
@@ -2357,16 +2357,16 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>15</v>
+        <v>276</v>
       </c>
     </row>
     <row r="85">
@@ -2385,11 +2385,11 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86">
@@ -2408,11 +2408,11 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>OUTRAS</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>157</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
@@ -2426,16 +2426,16 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>276</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88">
@@ -2454,11 +2454,11 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>124</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89">
@@ -2477,11 +2477,11 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>89</v>
+        <v>44</v>
       </c>
     </row>
     <row r="90">
@@ -2500,11 +2500,11 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>44</v>
+        <v>124</v>
       </c>
     </row>
     <row r="91">
@@ -2523,11 +2523,11 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>7</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92">
@@ -2564,16 +2564,16 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>21</v>
+        <v>333</v>
       </c>
     </row>
     <row r="94">
@@ -2592,11 +2592,11 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>10</v>
+        <v>75</v>
       </c>
     </row>
     <row r="95">
@@ -2615,11 +2615,11 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>333</v>
+        <v>83</v>
       </c>
     </row>
     <row r="96">
@@ -2638,11 +2638,11 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>75</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97">
@@ -2656,16 +2656,16 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>83</v>
+        <v>21</v>
       </c>
     </row>
     <row r="98">
@@ -2684,11 +2684,11 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>OFICIAL</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>724</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99">
@@ -2707,11 +2707,11 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>PRAÇA</t>
+          <t>OFICIAL</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>5145</v>
+        <v>724</v>
       </c>
     </row>
     <row r="100">
@@ -2725,16 +2725,16 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>INATIVO MILITAR</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>22</v>
+        <v>3219</v>
       </c>
     </row>
     <row r="101">
@@ -2753,11 +2753,11 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>PRAÇA</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>2</v>
+        <v>5145</v>
       </c>
     </row>
     <row r="102">
@@ -2771,16 +2771,16 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>INATIVO MILITAR</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>3219</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103">
@@ -2794,16 +2794,16 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E103" t="n">
-        <v>6</v>
+        <v>397</v>
       </c>
     </row>
     <row r="104">
@@ -2817,16 +2817,16 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E104" t="n">
-        <v>397</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105">
@@ -2868,11 +2868,11 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E106" t="n">
-        <v>114</v>
+        <v>983</v>
       </c>
     </row>
     <row r="107">
@@ -2891,11 +2891,11 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E107" t="n">
-        <v>983</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108">
@@ -2914,11 +2914,11 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E108" t="n">
-        <v>5</v>
+        <v>114</v>
       </c>
     </row>
     <row r="109">
@@ -2932,16 +2932,16 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E109" t="n">
-        <v>804</v>
+        <v>830</v>
       </c>
     </row>
     <row r="110">
@@ -2955,16 +2955,16 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>830</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="111">
@@ -3006,11 +3006,11 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E112" t="n">
-        <v>1139</v>
+        <v>285</v>
       </c>
     </row>
     <row r="113">
@@ -3029,11 +3029,11 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>NATUREZA ESPECIAL</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E113" t="n">
-        <v>3</v>
+        <v>17855</v>
       </c>
     </row>
     <row r="114">
@@ -3052,11 +3052,11 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>NATUREZA ESPECIAL</t>
         </is>
       </c>
       <c r="E114" t="n">
-        <v>17855</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115">
@@ -3075,11 +3075,11 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E115" t="n">
-        <v>285</v>
+        <v>804</v>
       </c>
     </row>
     <row r="116">
@@ -3093,16 +3093,16 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>DOCENTE</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E116" t="n">
-        <v>2</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="117">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E117" t="n">
@@ -3139,16 +3139,16 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E118" t="n">
-        <v>1151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="119">
@@ -3167,11 +3167,11 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E119" t="n">
-        <v>147</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -3236,11 +3236,11 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>DOCENTE</t>
         </is>
       </c>
       <c r="E122" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123">
@@ -3259,11 +3259,11 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E123" t="n">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="124">
@@ -3277,16 +3277,16 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E124" t="n">
-        <v>1073</v>
+        <v>262</v>
       </c>
     </row>
     <row r="125">
@@ -3305,11 +3305,11 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E125" t="n">
-        <v>63</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126">
@@ -3323,16 +3323,16 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E126" t="n">
-        <v>262</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="127">
@@ -3351,11 +3351,11 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="128">
@@ -3374,11 +3374,11 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>624</v>
+        <v>751</v>
       </c>
     </row>
     <row r="129">
@@ -3397,11 +3397,11 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E129" t="n">
-        <v>751</v>
+        <v>624</v>
       </c>
     </row>
     <row r="130">
@@ -3438,16 +3438,16 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E131" t="n">
-        <v>1067</v>
+        <v>7354</v>
       </c>
     </row>
     <row r="132">
@@ -3461,16 +3461,16 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>OUTRAS</t>
         </is>
       </c>
       <c r="E132" t="n">
-        <v>7354</v>
+        <v>10080</v>
       </c>
     </row>
     <row r="133">
@@ -3489,11 +3489,11 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>OUTRAS</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E133" t="n">
-        <v>10080</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="134">
@@ -3507,16 +3507,16 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E134" t="n">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="135">
@@ -3535,11 +3535,11 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E135" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="136">
@@ -3553,16 +3553,16 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E136" t="n">
-        <v>135</v>
+        <v>34</v>
       </c>
     </row>
     <row r="137">
@@ -3581,11 +3581,11 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>19</v>
+        <v>135</v>
       </c>
     </row>
     <row r="138">
@@ -3604,11 +3604,11 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E138" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139">
@@ -3645,16 +3645,16 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E140" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="141">
@@ -3696,11 +3696,11 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E142" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
@@ -3714,16 +3714,16 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E143" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144">
@@ -3742,11 +3742,11 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>ADMINISTRATIVA</t>
         </is>
       </c>
       <c r="E144" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145">
@@ -3765,11 +3765,11 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>ADMINISTRATIVA</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E145" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146">
@@ -3788,11 +3788,11 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E146" t="n">
-        <v>32</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147">
@@ -3811,11 +3811,11 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>MEMBROS DE PODER</t>
         </is>
       </c>
       <c r="E147" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148">
@@ -3834,11 +3834,11 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>MEMBROS DE PODER</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E148" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="149">
@@ -3903,11 +3903,11 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E151" t="n">
-        <v>91</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152">
@@ -3926,11 +3926,11 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E152" t="n">
-        <v>2</v>
+        <v>91</v>
       </c>
     </row>
     <row r="153">
@@ -3949,11 +3949,11 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>DIREÇÃO SUPERIOR</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E153" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154">
@@ -3972,11 +3972,11 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>DIREÇÃO SUPERIOR</t>
         </is>
       </c>
       <c r="E154" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155">
@@ -3995,11 +3995,11 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E155" t="n">
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="156">
@@ -4018,11 +4018,11 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E156" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157">
@@ -7918,7 +7918,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>4031 - FEPJ</t>
+          <t>4291 - FES</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -7932,7 +7932,7 @@
         </is>
       </c>
       <c r="E326" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="327">
@@ -7941,7 +7941,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>4031 - FEPJ</t>
+          <t>4291 - FES</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -7951,11 +7951,11 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>ESPECIALIZADA</t>
+          <t>DIREÇÃO E ASSESSORAMENTO</t>
         </is>
       </c>
       <c r="E327" t="n">
-        <v>1161</v>
+        <v>84</v>
       </c>
     </row>
     <row r="328">
@@ -7964,21 +7964,21 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>4031 - FEPJ</t>
+          <t>4291 - FES</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>Inativo</t>
+          <t>Ativo</t>
         </is>
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>INATIVO CIVIL</t>
+          <t>TÉCNICA</t>
         </is>
       </c>
       <c r="E328" t="n">
-        <v>6977</v>
+        <v>250</v>
       </c>
     </row>
     <row r="329">
@@ -7987,21 +7987,21 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>4031 - FEPJ</t>
+          <t>4291 - FES</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>Ativo</t>
+          <t>Inativo</t>
         </is>
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>MEMBROS DE PODER</t>
+          <t>INATIVO CIVIL</t>
         </is>
       </c>
       <c r="E329" t="n">
-        <v>1132</v>
+        <v>8614</v>
       </c>
     </row>
     <row r="330">
@@ -8010,7 +8010,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>4031 - FEPJ</t>
+          <t>4291 - FES</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -8024,7 +8024,7 @@
         </is>
       </c>
       <c r="E330" t="n">
-        <v>8557</v>
+        <v>949</v>
       </c>
     </row>
     <row r="331">
@@ -8033,7 +8033,7 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>4031 - FEPJ</t>
+          <t>4291 - FES</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -8043,11 +8043,11 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>TÉCNICA</t>
+          <t>OUTRAS</t>
         </is>
       </c>
       <c r="E331" t="n">
-        <v>110</v>
+        <v>449</v>
       </c>
     </row>
     <row r="332">
@@ -8056,7 +8056,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>4031 - FEPJ</t>
+          <t>4291 - FES</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -8066,172 +8066,11 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
+          <t>ESPECIALIZADA</t>
         </is>
       </c>
       <c r="E332" t="n">
-        <v>3765</v>
-      </c>
-    </row>
-    <row r="333">
-      <c r="A333" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B333" t="inlineStr">
-        <is>
-          <t>4291 - FES</t>
-        </is>
-      </c>
-      <c r="C333" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="D333" t="inlineStr">
-        <is>
-          <t>ESPECIALIZADA</t>
-        </is>
-      </c>
-      <c r="E333" t="n">
         <v>1925</v>
-      </c>
-    </row>
-    <row r="334">
-      <c r="A334" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B334" t="inlineStr">
-        <is>
-          <t>4291 - FES</t>
-        </is>
-      </c>
-      <c r="C334" t="inlineStr">
-        <is>
-          <t>Inativo</t>
-        </is>
-      </c>
-      <c r="D334" t="inlineStr">
-        <is>
-          <t>INATIVO CIVIL</t>
-        </is>
-      </c>
-      <c r="E334" t="n">
-        <v>8614</v>
-      </c>
-    </row>
-    <row r="335">
-      <c r="A335" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B335" t="inlineStr">
-        <is>
-          <t>4291 - FES</t>
-        </is>
-      </c>
-      <c r="C335" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="D335" t="inlineStr">
-        <is>
-          <t>TÉCNICA</t>
-        </is>
-      </c>
-      <c r="E335" t="n">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="336">
-      <c r="A336" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B336" t="inlineStr">
-        <is>
-          <t>4291 - FES</t>
-        </is>
-      </c>
-      <c r="C336" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="D336" t="inlineStr">
-        <is>
-          <t>ADMINISTRATIVA</t>
-        </is>
-      </c>
-      <c r="E336" t="n">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="337">
-      <c r="A337" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B337" t="inlineStr">
-        <is>
-          <t>4291 - FES</t>
-        </is>
-      </c>
-      <c r="C337" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="D337" t="inlineStr">
-        <is>
-          <t>DIREÇÃO E ASSESSORAMENTO</t>
-        </is>
-      </c>
-      <c r="E337" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="338">
-      <c r="A338" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B338" t="inlineStr">
-        <is>
-          <t>4291 - FES</t>
-        </is>
-      </c>
-      <c r="C338" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="D338" t="inlineStr">
-        <is>
-          <t>OUTRAS</t>
-        </is>
-      </c>
-      <c r="E338" t="n">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="339">
-      <c r="A339" t="n">
-        <v>2026</v>
-      </c>
-      <c r="B339" t="inlineStr">
-        <is>
-          <t>4291 - FES</t>
-        </is>
-      </c>
-      <c r="C339" t="inlineStr">
-        <is>
-          <t>Ativo</t>
-        </is>
-      </c>
-      <c r="D339" t="inlineStr">
-        <is>
-          <t>DIREÇÃO SUPERIOR</t>
-        </is>
-      </c>
-      <c r="E339" t="n">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>